<commit_message>
Modele de bilan en liste avant répartition par ANC
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/1_Bilan/Bilan.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/1_Bilan/Bilan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="151">
   <si>
     <t>Modèle de bilan en tableau</t>
   </si>
@@ -356,6 +356,135 @@
   </si>
   <si>
     <t>(f) A l'exception, pour l'application du (1), des avances et acomptes reçus sur commandes en cours.</t>
+  </si>
+  <si>
+    <t>Modèle de bilan en liste avant répartition</t>
+  </si>
+  <si>
+    <t>ACTIF</t>
+  </si>
+  <si>
+    <t>ACTIF IMMOBILISE (b)</t>
+  </si>
+  <si>
+    <t>Participations ('c')</t>
+  </si>
+  <si>
+    <t>(a) Pour la présentation de la situation nette, après répartition, le modèle est modifié en conséquence.</t>
+  </si>
+  <si>
+    <t>(b) Les actifs avec clause de réserve de propriété sont regroupés sur une ligne distincte portant la mention “ dont
+...€ avec clause de réserve de propriété ”. En cas d’impossibilité d’identifier les biens, un renvoi au pied du bilan
+indique le montant restant à payer sur ces biens. Le montant à payer comprend celui des effets non échus.</t>
+  </si>
+  <si>
+    <t>(c) Si des titres sont évalués par équivalence, ce poste est subdivisé en deux sous-postes “ Participations
+évaluées par équivalence ” et “ Autres participations ”. Pour les titres évalués par équivalence, la colonne “ Brut ”
+présente la valeur globale d’équivalence si elle est supérieure au coût d’acquisition. Dans le cas contraire, le prix
+d’acquisition est retenu. La dépréciation globale du portefeuille figure dans la 2ème colonne. La colonne “ Net ”
+présente la valeur globale d’équivalence positive ou une valeur nulle.</t>
+  </si>
+  <si>
+    <t>Stocks et en-cours (b) :</t>
+  </si>
+  <si>
+    <t>En-cours de production [biens et services] (d)</t>
+  </si>
+  <si>
+    <t>Créances Clients (b) et Comptes rattachés ('e')</t>
+  </si>
+  <si>
+    <t>Valeurs mobilières de placement (f) :</t>
+  </si>
+  <si>
+    <t>TOTAL ACTIF VI (I + II + III + IV +V).....</t>
+  </si>
+  <si>
+    <t>(3) Dont à plus d’un an (brut)</t>
+  </si>
+  <si>
+    <t>(d) A ventiler, le cas échéant, entre biens, d'une part, et services d'autre part.</t>
+  </si>
+  <si>
+    <t>(e) Créances résultant de ventes ou de prestations de services.</t>
+  </si>
+  <si>
+    <t>(f) Poste à servir directement s'il n'existe pas de rachat par l’entité de ses propres actions.</t>
+  </si>
+  <si>
+    <t>DETTES A MOINS D'UN AN</t>
+  </si>
+  <si>
+    <t>Emprunts et dettes auprès des établissements de crédit (4)</t>
+  </si>
+  <si>
+    <t>Emprunts et dettes financières divers</t>
+  </si>
+  <si>
+    <t>Dettes Fournisseurs et Comptes rattachés (g)</t>
+  </si>
+  <si>
+    <t>Produits constatés d’avance</t>
+  </si>
+  <si>
+    <t>Excédent de l'actif circulant sur les dettes à moins d'un an (II- VII)</t>
+  </si>
+  <si>
+    <t>Excédent de l'actif sur les dettes à moins d'un an (VI - VII)</t>
+  </si>
+  <si>
+    <t>Total (VII)</t>
+  </si>
+  <si>
+    <t>DETTES A PLUS D'UN AN</t>
+  </si>
+  <si>
+    <t>Total (VIII)</t>
+  </si>
+  <si>
+    <t>Ecarts de conversion et différences d’évaluation Passif (IX)</t>
+  </si>
+  <si>
+    <t>Total (X)</t>
+  </si>
+  <si>
+    <t>(4) Dont concours bancaires courants et soldes créditeurs de banques</t>
+  </si>
+  <si>
+    <t>CAPITAUX PROPRES</t>
+  </si>
+  <si>
+    <t>Capital [dont versé...]</t>
+  </si>
+  <si>
+    <t>Ecarts de réévaluation (h)</t>
+  </si>
+  <si>
+    <t>Ecart d’équivalence (i)</t>
+  </si>
+  <si>
+    <t>Report à nouveau (j)</t>
+  </si>
+  <si>
+    <t>Résultat de l'exercice [bénéfice ou perte] (k)</t>
+  </si>
+  <si>
+    <t>Total (XI) ou [VI - (VII + VIII + IX + X)]</t>
+  </si>
+  <si>
+    <t>(g) Dettes sur achats et prestations de services.</t>
+  </si>
+  <si>
+    <t>(h) A détailler conformément à la législation en vigueur.</t>
+  </si>
+  <si>
+    <t>(i) Poste à présenter lorsque des titres sont évalués par équivalence.</t>
+  </si>
+  <si>
+    <t>(j) Montant entre parenthèses ou précédé du signe moins (-) lorsqu'il s'agit de pertes reportées.</t>
+  </si>
+  <si>
+    <t>(k) Montant entre parenthèses ou précédés du signe moins (-) lorsqu’il s’agit d’une perte.</t>
   </si>
 </sst>
 </file>
@@ -533,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,6 +755,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
@@ -931,17 +1088,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:E277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
+      <selection activeCell="A286" sqref="A286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.28515625" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -977,16 +1134,16 @@
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1071,8 +1228,8 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="12"/>
@@ -1330,16 +1487,16 @@
       <c r="A36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2279,7 +2436,7 @@
       <c r="B144" s="17"/>
       <c r="C144" s="17"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="16" t="s">
         <v>89</v>
       </c>
@@ -2292,65 +2449,1208 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="20" t="s">
         <v>90</v>
       </c>
       <c r="B146" s="35"/>
       <c r="C146" s="35"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="20" t="s">
         <v>91</v>
       </c>
       <c r="B147" s="35"/>
       <c r="C147" s="35"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
         <v>92</v>
       </c>
       <c r="B148" s="35"/>
       <c r="C148" s="35"/>
     </row>
-    <row r="149" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A149" s="23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="23" t="s">
         <v>109</v>
       </c>
     </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="40"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B158" s="41"/>
+      <c r="C158" s="41"/>
+      <c r="D158" s="41"/>
+      <c r="E158" s="38"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B160" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C160" s="39"/>
+      <c r="D160" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E160" s="39"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B161" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D161" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E161" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" s="10"/>
+      <c r="C162" s="10"/>
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B163" s="10">
+        <f>SUM(B164,B172,B179)</f>
+        <v>0</v>
+      </c>
+      <c r="C163" s="10">
+        <f>SUM(C164,C172,C179)</f>
+        <v>0</v>
+      </c>
+      <c r="D163" s="10">
+        <f>SUM(D164,D172,D179)</f>
+        <v>0</v>
+      </c>
+      <c r="E163" s="10">
+        <f>SUM(E164,E172,E179)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B164" s="11">
+        <f>SUM(B165:B171)</f>
+        <v>0</v>
+      </c>
+      <c r="C164" s="11">
+        <f>SUM(C165:C171)</f>
+        <v>0</v>
+      </c>
+      <c r="D164" s="11">
+        <f t="shared" ref="D164:E164" si="8">SUM(D165:D171)</f>
+        <v>0</v>
+      </c>
+      <c r="E164" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165" s="12"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="12"/>
+      <c r="E165" s="12"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B166" s="12"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="12"/>
+      <c r="E166" s="12"/>
+    </row>
+    <row r="167" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A167" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B167" s="12"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="12"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B168" s="12"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B169" s="12"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="12"/>
+      <c r="E169" s="12"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B170" s="12"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="12"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B171" s="12"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="12"/>
+      <c r="E171" s="12"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B172" s="11">
+        <f>SUM(B173:B178)</f>
+        <v>0</v>
+      </c>
+      <c r="C172" s="11">
+        <f t="shared" ref="C172:E172" si="9">SUM(C173:C178)</f>
+        <v>0</v>
+      </c>
+      <c r="D172" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E172" s="11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B173" s="12"/>
+      <c r="C173" s="12"/>
+      <c r="D173" s="12"/>
+      <c r="E173" s="12"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B174" s="12"/>
+      <c r="C174" s="12"/>
+      <c r="D174" s="12"/>
+      <c r="E174" s="12"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B175" s="12"/>
+      <c r="C175" s="12"/>
+      <c r="D175" s="12"/>
+      <c r="E175" s="12"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B176" s="12"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="12"/>
+      <c r="E176" s="12"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B177" s="12"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="12"/>
+      <c r="E177" s="12"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B178" s="12"/>
+      <c r="C178" s="12"/>
+      <c r="D178" s="12"/>
+      <c r="E178" s="12"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B179" s="11">
+        <f>SUM(B180:B185)</f>
+        <v>0</v>
+      </c>
+      <c r="C179" s="11">
+        <f t="shared" ref="C179:D179" si="10">SUM(C180:C185)</f>
+        <v>0</v>
+      </c>
+      <c r="D179" s="11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E179" s="11">
+        <f>SUM(E180:E185)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B180" s="12"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B181" s="12"/>
+      <c r="C181" s="12"/>
+      <c r="D181" s="12"/>
+      <c r="E181" s="12"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B182" s="12"/>
+      <c r="C182" s="12"/>
+      <c r="D182" s="12"/>
+      <c r="E182" s="12"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B183" s="12"/>
+      <c r="C183" s="12"/>
+      <c r="D183" s="12"/>
+      <c r="E183" s="12"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B184" s="12"/>
+      <c r="C184" s="12"/>
+      <c r="D184" s="12"/>
+      <c r="E184" s="12"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B185" s="12"/>
+      <c r="C185" s="12"/>
+      <c r="D185" s="12"/>
+      <c r="E185" s="12"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B186" s="18">
+        <f>SUM(B162:B163)</f>
+        <v>0</v>
+      </c>
+      <c r="C186" s="18">
+        <f>SUM(C162:C163)</f>
+        <v>0</v>
+      </c>
+      <c r="D186" s="18">
+        <f>SUM(D162:D163)</f>
+        <v>0</v>
+      </c>
+      <c r="E186" s="18">
+        <f>SUM(E162:E163)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B187" s="31"/>
+      <c r="C187" s="32"/>
+      <c r="D187" s="35"/>
+      <c r="E187" s="35"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B188" s="31"/>
+      <c r="C188" s="32"/>
+      <c r="D188" s="35"/>
+      <c r="E188" s="35"/>
+    </row>
+    <row r="189" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A189" s="23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A190" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A191" s="23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B193" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C193" s="39"/>
+      <c r="D193" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E193" s="39"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B194" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C194" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D194" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E194" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B195" s="10">
+        <f>SUM(B196,B202,B206)</f>
+        <v>0</v>
+      </c>
+      <c r="C195" s="10">
+        <f>SUM(C196,C202,C206)</f>
+        <v>0</v>
+      </c>
+      <c r="D195" s="10">
+        <f>SUM(D196,D202,D206)</f>
+        <v>0</v>
+      </c>
+      <c r="E195" s="10">
+        <f>SUM(E196,E202,E206)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B196" s="11">
+        <f>SUM(B197:B201)</f>
+        <v>0</v>
+      </c>
+      <c r="C196" s="11">
+        <f>SUM(C197:C201)</f>
+        <v>0</v>
+      </c>
+      <c r="D196" s="11">
+        <f>SUM(D197:D201)</f>
+        <v>0</v>
+      </c>
+      <c r="E196" s="11">
+        <f>SUM(E197:E201)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B197" s="12"/>
+      <c r="C197" s="12"/>
+      <c r="D197" s="12"/>
+      <c r="E197" s="12"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B198" s="12"/>
+      <c r="C198" s="12"/>
+      <c r="D198" s="12"/>
+      <c r="E198" s="12"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B199" s="12"/>
+      <c r="C199" s="12"/>
+      <c r="D199" s="12"/>
+      <c r="E199" s="12"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B200" s="12"/>
+      <c r="C200" s="12"/>
+      <c r="D200" s="12"/>
+      <c r="E200" s="12"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B201" s="12"/>
+      <c r="C201" s="12"/>
+      <c r="D201" s="12"/>
+      <c r="E201" s="12"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B202" s="11">
+        <f>SUM(B203:B205)</f>
+        <v>0</v>
+      </c>
+      <c r="C202" s="11">
+        <f>SUM(C203:C205)</f>
+        <v>0</v>
+      </c>
+      <c r="D202" s="11">
+        <f>SUM(D203:D205)</f>
+        <v>0</v>
+      </c>
+      <c r="E202" s="11">
+        <f>SUM(E203:E205)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B203" s="12"/>
+      <c r="C203" s="12"/>
+      <c r="D203" s="12"/>
+      <c r="E203" s="12"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B204" s="12"/>
+      <c r="C204" s="12"/>
+      <c r="D204" s="12"/>
+      <c r="E204" s="12"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B205" s="12"/>
+      <c r="C205" s="12"/>
+      <c r="D205" s="12"/>
+      <c r="E205" s="12"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B206" s="11">
+        <f>SUM(B207:B211)</f>
+        <v>0</v>
+      </c>
+      <c r="C206" s="11">
+        <f>SUM(C207:C211)</f>
+        <v>0</v>
+      </c>
+      <c r="D206" s="11">
+        <f>SUM(D207:D211)</f>
+        <v>0</v>
+      </c>
+      <c r="E206" s="11">
+        <f>SUM(E207:E211)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B207" s="12"/>
+      <c r="C207" s="12"/>
+      <c r="D207" s="12"/>
+      <c r="E207" s="12"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B208" s="12"/>
+      <c r="C208" s="12"/>
+      <c r="D208" s="12"/>
+      <c r="E208" s="12"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B209" s="12"/>
+      <c r="C209" s="12"/>
+      <c r="D209" s="12"/>
+      <c r="E209" s="12"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B210" s="12"/>
+      <c r="C210" s="12"/>
+      <c r="D210" s="12"/>
+      <c r="E210" s="12"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B211" s="12"/>
+      <c r="C211" s="12"/>
+      <c r="D211" s="12"/>
+      <c r="E211" s="12"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B212" s="18">
+        <f>B195</f>
+        <v>0</v>
+      </c>
+      <c r="C212" s="18">
+        <f>C195</f>
+        <v>0</v>
+      </c>
+      <c r="D212" s="18">
+        <f>D195</f>
+        <v>0</v>
+      </c>
+      <c r="E212" s="18">
+        <f>E195</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B213" s="16"/>
+      <c r="C213" s="16"/>
+      <c r="D213" s="16"/>
+      <c r="E213" s="16"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B214" s="16"/>
+      <c r="C214" s="43"/>
+      <c r="D214" s="16"/>
+      <c r="E214" s="16"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B215" s="16"/>
+      <c r="C215" s="43"/>
+      <c r="D215" s="16"/>
+      <c r="E215" s="16"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B216" s="26">
+        <f>SUM(B212:B215,B186)</f>
+        <v>0</v>
+      </c>
+      <c r="C216" s="26">
+        <f>SUM(C212:C213,C186)</f>
+        <v>0</v>
+      </c>
+      <c r="D216" s="26">
+        <f>SUM(D212:D215,D186)</f>
+        <v>0</v>
+      </c>
+      <c r="E216" s="26">
+        <f>SUM(E212:E215,E186)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B217" s="31"/>
+      <c r="C217" s="32"/>
+      <c r="D217" s="20"/>
+      <c r="E217" s="20"/>
+    </row>
+    <row r="218" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A218" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A220" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="2"/>
+      <c r="B222" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C222" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B223" s="10">
+        <f>SUM(B224:B234)</f>
+        <v>0</v>
+      </c>
+      <c r="C223" s="10">
+        <f>SUM(C224:C234)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B224" s="11"/>
+      <c r="C224" s="11"/>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B225" s="11"/>
+      <c r="C225" s="11"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B226" s="11"/>
+      <c r="C226" s="11"/>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B227" s="11"/>
+      <c r="C227" s="11"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B228" s="11"/>
+      <c r="C228" s="11"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B229" s="11"/>
+      <c r="C229" s="11"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B230" s="11"/>
+      <c r="C230" s="11"/>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B231" s="11"/>
+      <c r="C231" s="11"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B232" s="11"/>
+      <c r="C232" s="11"/>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B233" s="11"/>
+      <c r="C233" s="11"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B234" s="11"/>
+      <c r="C234" s="11"/>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B235" s="18">
+        <f>B223</f>
+        <v>0</v>
+      </c>
+      <c r="C235" s="18">
+        <f>C223</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B236" s="26">
+        <f>B212-B235</f>
+        <v>0</v>
+      </c>
+      <c r="C236" s="26">
+        <f>C212-C235</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B237" s="26">
+        <f>B216-B235</f>
+        <v>0</v>
+      </c>
+      <c r="C237" s="26">
+        <f>C216-C235</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B238" s="10">
+        <f>SUM(B239:B249)</f>
+        <v>0</v>
+      </c>
+      <c r="C238" s="10">
+        <f>SUM(C239:C249)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B239" s="11"/>
+      <c r="C239" s="11"/>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B240" s="11"/>
+      <c r="C240" s="11"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B241" s="11"/>
+      <c r="C241" s="11"/>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B242" s="11"/>
+      <c r="C242" s="11"/>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B243" s="11"/>
+      <c r="C243" s="11"/>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B244" s="11"/>
+      <c r="C244" s="11"/>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B245" s="11"/>
+      <c r="C245" s="11"/>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B246" s="11"/>
+      <c r="C246" s="11"/>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B247" s="11"/>
+      <c r="C247" s="11"/>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B248" s="11"/>
+      <c r="C248" s="11"/>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B249" s="11"/>
+      <c r="C249" s="11"/>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B250" s="18">
+        <f>B238</f>
+        <v>0</v>
+      </c>
+      <c r="C250" s="18">
+        <f>C238</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B251" s="18"/>
+      <c r="C251" s="18"/>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B252" s="25">
+        <f>SUM(B253:B254)</f>
+        <v>0</v>
+      </c>
+      <c r="C252" s="25">
+        <f>SUM(C253:C254)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B253" s="11"/>
+      <c r="C253" s="11"/>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B254" s="11"/>
+      <c r="C254" s="11"/>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="B255" s="18">
+        <f>B252</f>
+        <v>0</v>
+      </c>
+      <c r="C255" s="18">
+        <f>C252</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B256" s="20"/>
+      <c r="C256" s="20"/>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B257" s="10">
+        <f>SUM(B258:B262)</f>
+        <v>0</v>
+      </c>
+      <c r="C257" s="10">
+        <f>SUM(C258:C262)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B258" s="11"/>
+      <c r="C258" s="11"/>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B259" s="11"/>
+      <c r="C259" s="11"/>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B260" s="11"/>
+      <c r="C260" s="11"/>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B261" s="11"/>
+      <c r="C261" s="11"/>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B262" s="11">
+        <f>SUM(B263:B270)</f>
+        <v>0</v>
+      </c>
+      <c r="C262" s="11">
+        <f>SUM(C263:C270)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B263" s="12"/>
+      <c r="C263" s="12"/>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B264" s="12"/>
+      <c r="C264" s="12"/>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B265" s="12"/>
+      <c r="C265" s="12"/>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B266" s="12"/>
+      <c r="C266" s="12"/>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B267" s="12"/>
+      <c r="C267" s="12"/>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B268" s="12"/>
+      <c r="C268" s="12"/>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B269" s="12"/>
+      <c r="C269" s="12"/>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B270" s="12"/>
+      <c r="C270" s="12"/>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B271" s="18">
+        <f>B216-(B235+B250+B251+B255)</f>
+        <v>0</v>
+      </c>
+      <c r="C271" s="18">
+        <f>C216-(C235+C250+C251+C255)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="B272" s="13"/>
+      <c r="C272" s="13"/>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B273" s="13"/>
+      <c r="C273" s="13"/>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B274" s="13"/>
+      <c r="C274" s="13"/>
+    </row>
+    <row r="275" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A275" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="B275" s="13"/>
+      <c r="C275" s="13"/>
+    </row>
+    <row r="276" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A276" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B276" s="13"/>
+      <c r="C276" s="13"/>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B277" s="44"/>
+      <c r="C277" s="44"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="14">
+    <mergeCell ref="A187:C187"/>
+    <mergeCell ref="A188:C188"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="D193:E193"/>
+    <mergeCell ref="A217:C217"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="A158:E158"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="A30:C30"/>

</xml_diff>

<commit_message>
Bilan _ Systeme developpe
</commit_message>
<xml_diff>
--- a/France/3_Comptabilite_Et_Fiscalite/1_Bilan/Bilan.xlsx
+++ b/France/3_Comptabilite_Et_Fiscalite/1_Bilan/Bilan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Systeme_De_Base" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="213">
   <si>
     <t>Modèle de bilan en tableau</t>
   </si>
@@ -634,6 +634,62 @@
   </si>
   <si>
     <t>Sous total : situation nette</t>
+  </si>
+  <si>
+    <t>Modèle de bilan</t>
+  </si>
+  <si>
+    <t>Concessions, brevets, licences, marques,
+procédés, logiciels, droits et valeurs similaires</t>
+  </si>
+  <si>
+    <t>(2) Dont à moins d’un an</t>
+  </si>
+  <si>
+    <t>(b) Si des titres sont évalués par équivalence, ce poste est subdivisé en deux sous-postes “ Participations
+évaluées par équivalence ” et “ Autres participations ”. Pour les titres évalués par équivalence, la colonne “ Brut ”
+présente la valeur globale d’équivalence si elle est supérieure au coût d’acquisition. Dans le cas contraire, le prix
+d’acquisition est retenu. La dépréciation globale du portefeuille figure dans la 2ème colonne. La colonne “ Net ”
+présente la valeur globale d’équivalence positive ou une valeur nulle.</t>
+  </si>
+  <si>
+    <t>ACTIF (suite)</t>
+  </si>
+  <si>
+    <t>Créances d’exploitation (3) :</t>
+  </si>
+  <si>
+    <t>Créances Clients et Comptes rattachés (a) (d)</t>
+  </si>
+  <si>
+    <t>TOTAL GENERAL (I + II + III + IV + V)</t>
+  </si>
+  <si>
+    <t>(3) Dont à plus d’un an</t>
+  </si>
+  <si>
+    <t>Dettes financières :</t>
+  </si>
+  <si>
+    <t>Dettes d'exploitation :</t>
+  </si>
+  <si>
+    <t>Dettes diverses :</t>
+  </si>
+  <si>
+    <t>Dettes fiscales (impôts sur les bénéfices)</t>
+  </si>
+  <si>
+    <t>* Le cas échéant, une rubrique "Autres fonds propres" est intercalée entre la rubrique "Capitaux propres" et la rubrique
+"Provisions " avec ouverture des postes constitutifs de cette rubrique sur des lignes séparées (montant des émissions de titres
+participatifs, avances conditionnées, ...). Un total I bis fait apparaître le montant des autres fonds propres entre le total I et le
+total II du passif du bilan. Le total général est complété en conséquence.</t>
+  </si>
+  <si>
+    <t>(e) Montant entre parenthèses ou précédé du signe moins (-) lorsqu'il s'agit d'une perte.</t>
+  </si>
+  <si>
+    <t>Produits constatés d'avance</t>
   </si>
 </sst>
 </file>
@@ -727,7 +783,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -814,8 +870,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -827,7 +905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -918,19 +996,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -943,6 +1028,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -966,35 +1078,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1317,13 +1414,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -1334,11 +1431,11 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="1" t="s">
         <v>71</v>
       </c>
@@ -1658,20 +1755,20 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
     </row>
@@ -1687,11 +1784,11 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
-      <c r="B35" s="44" t="s">
+      <c r="B35" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
       <c r="E35" s="1" t="s">
         <v>71</v>
       </c>
@@ -1984,11 +2081,11 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="37"/>
-      <c r="C59" s="38"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
     </row>
@@ -2722,23 +2819,23 @@
       <c r="A156" s="31"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="41" t="s">
+      <c r="A158" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="B158" s="42"/>
-      <c r="C158" s="42"/>
-      <c r="D158" s="42"/>
-      <c r="E158" s="43"/>
+      <c r="B158" s="45"/>
+      <c r="C158" s="45"/>
+      <c r="D158" s="45"/>
+      <c r="E158" s="46"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B160" s="39" t="s">
+      <c r="B160" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C160" s="39"/>
-      <c r="D160" s="39" t="s">
+      <c r="C160" s="43"/>
+      <c r="D160" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E160" s="39"/>
+      <c r="E160" s="43"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="22" t="s">
@@ -3043,20 +3140,20 @@
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="36" t="s">
+      <c r="A187" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B187" s="37"/>
-      <c r="C187" s="38"/>
+      <c r="B187" s="49"/>
+      <c r="C187" s="50"/>
       <c r="D187" s="28"/>
       <c r="E187" s="28"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="36" t="s">
+      <c r="A188" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B188" s="37"/>
-      <c r="C188" s="38"/>
+      <c r="B188" s="49"/>
+      <c r="C188" s="50"/>
       <c r="D188" s="28"/>
       <c r="E188" s="28"/>
     </row>
@@ -3076,14 +3173,14 @@
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B193" s="39" t="s">
+      <c r="B193" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C193" s="39"/>
-      <c r="D193" s="39" t="s">
+      <c r="C193" s="43"/>
+      <c r="D193" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E193" s="39"/>
+      <c r="E193" s="43"/>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="29" t="s">
@@ -3373,11 +3470,11 @@
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" s="36" t="s">
+      <c r="A217" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="B217" s="37"/>
-      <c r="C217" s="38"/>
+      <c r="B217" s="49"/>
+      <c r="C217" s="50"/>
       <c r="D217" s="18"/>
       <c r="E217" s="18"/>
     </row>
@@ -3855,6 +3952,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A187:C187"/>
+    <mergeCell ref="A188:C188"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="D193:E193"/>
+    <mergeCell ref="A217:C217"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D160:E160"/>
     <mergeCell ref="B160:C160"/>
@@ -3864,11 +3966,6 @@
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A187:C187"/>
-    <mergeCell ref="A188:C188"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="D193:E193"/>
-    <mergeCell ref="A217:C217"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3879,8 +3976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,41 +3993,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="43" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
@@ -3943,9 +4040,9 @@
       <c r="E4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="39"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -4302,21 +4399,21 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="37" t="s">
         <v>168</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
-      <c r="F23" s="52" t="s">
+      <c r="F23" s="37" t="s">
         <v>186</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="52" t="s">
+      <c r="A24" s="37" t="s">
         <v>169</v>
       </c>
       <c r="B24" s="16">
@@ -4335,7 +4432,7 @@
         <f>SUM(E22:E23,E11)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="52" t="s">
+      <c r="F24" s="37" t="s">
         <v>187</v>
       </c>
       <c r="G24" s="16">
@@ -4348,11 +4445,11 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="18" t="s">
@@ -4362,42 +4459,42 @@
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
-      <c r="F26" s="53" t="s">
+      <c r="F26" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="G26" s="56"/>
-      <c r="H26" s="57"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="55"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="59"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="56"/>
     </row>
     <row r="28" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
@@ -4420,34 +4517,41 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="64" t="s">
         <v>195</v>
       </c>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="61"/>
       <c r="E38" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="F38" s="50" t="s">
+      <c r="F38" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="G38" s="50" t="s">
+      <c r="G38" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H38" s="39" t="s">
+      <c r="H38" s="43" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
+      <c r="A39" s="58"/>
       <c r="B39" s="30" t="s">
         <v>2</v>
       </c>
@@ -4460,9 +4564,9 @@
       <c r="E39" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="39"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="43"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -4819,21 +4923,21 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="52" t="s">
+      <c r="A58" s="37" t="s">
         <v>168</v>
       </c>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
-      <c r="F58" s="52" t="s">
+      <c r="F58" s="37" t="s">
         <v>186</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="52" t="s">
+      <c r="A59" s="37" t="s">
         <v>169</v>
       </c>
       <c r="B59" s="16">
@@ -4852,7 +4956,7 @@
         <f>SUM(E57:E58,E46)</f>
         <v>0</v>
       </c>
-      <c r="F59" s="52" t="s">
+      <c r="F59" s="37" t="s">
         <v>187</v>
       </c>
       <c r="G59" s="16">
@@ -4865,11 +4969,11 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="B60" s="37"/>
-      <c r="C60" s="38"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="50"/>
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
       <c r="F60" s="18" t="s">
@@ -4879,30 +4983,30 @@
       <c r="H60" s="19"/>
     </row>
     <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="36" t="s">
+      <c r="A61" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="B61" s="37"/>
-      <c r="C61" s="38"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="50"/>
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
-      <c r="F61" s="53" t="s">
+      <c r="F61" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="G61" s="56"/>
-      <c r="H61" s="57"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="55"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="36" t="s">
+      <c r="A62" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="19"/>
       <c r="E62" s="19"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="59"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="54"/>
+      <c r="H62" s="56"/>
     </row>
     <row r="63" spans="1:8" ht="180" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
@@ -4930,30 +5034,31 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="H38:H39"/>
     <mergeCell ref="A60:C60"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="F61:F62"/>
     <mergeCell ref="G61:G62"/>
     <mergeCell ref="H61:H62"/>
     <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="A25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4961,12 +5066,1557 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="43"/>
+      <c r="B4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8">
+        <f>SUM(B7,B15,B22)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" ref="C6:E6" si="0">SUM(C7,C15,C22)</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9">
+        <f>SUM(B8:B14)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <f>SUM(C8:C14)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <f>SUM(D8:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <f>SUM(E8:E14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9">
+        <f>SUM(B16:B21)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="9">
+        <f>SUM(C16:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <f>SUM(D16:D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <f>SUM(E16:E21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="9">
+        <f>SUM(B23:B28)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="9">
+        <f>SUM(C23:C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <f>SUM(D23:D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <f>SUM(E23:E28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="16">
+        <f>SUM(B5:B6)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="16">
+        <f t="shared" ref="C29:E29" si="1">SUM(C5:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="48" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+    </row>
+    <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+    </row>
+    <row r="33" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="8">
+        <f>SUM(B38,B44,B48)</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="8">
+        <f>SUM(C38,C44,C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="8">
+        <f>SUM(D38,D44,D48)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="8">
+        <f>SUM(E38,E44,E48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="9">
+        <f>SUM(B39:B43)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="9">
+        <f t="shared" ref="C38:E38" si="2">SUM(C39:C43)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="9">
+        <f>SUM(B45:B47)</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="9">
+        <f t="shared" ref="C44:E44" si="3">SUM(C45:C47)</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="9">
+        <f>SUM(B49:B53)</f>
+        <v>0</v>
+      </c>
+      <c r="C48" s="9">
+        <f>SUM(C49:C53)</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="9">
+        <f>SUM(D49:D53)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="9">
+        <f>SUM(E49:E53)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="16">
+        <f>B37</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="16">
+        <f>C37</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="16">
+        <f>D37</f>
+        <v>0</v>
+      </c>
+      <c r="E54" s="16">
+        <f>E37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" s="15">
+        <f>SUM(B54:B57,B29)</f>
+        <v>0</v>
+      </c>
+      <c r="C58" s="15">
+        <f>SUM(C54:C57,C29)</f>
+        <v>0</v>
+      </c>
+      <c r="D58" s="15">
+        <f>SUM(D54:D57,D29)</f>
+        <v>0</v>
+      </c>
+      <c r="E58" s="15">
+        <f>SUM(E54:E57,E29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" s="8">
+        <f>SUM(B66:B70)</f>
+        <v>0</v>
+      </c>
+      <c r="C65" s="8">
+        <f>SUM(C66:C70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70" s="9">
+        <f>SUM(B71:B78)</f>
+        <v>0</v>
+      </c>
+      <c r="C70" s="9">
+        <f>SUM(C71:C78)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B79" s="16">
+        <f>B65</f>
+        <v>0</v>
+      </c>
+      <c r="C79" s="16">
+        <f>C65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="8">
+        <f>SUM(B81:B82)</f>
+        <v>0</v>
+      </c>
+      <c r="C80" s="8">
+        <f>SUM(C81:C82)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" s="16">
+        <f>B80</f>
+        <v>0</v>
+      </c>
+      <c r="C83" s="16">
+        <f>C80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B84" s="8">
+        <f>SUM(B85,B91,B95)</f>
+        <v>0</v>
+      </c>
+      <c r="C84" s="8">
+        <f>SUM(C85,C91,C95)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B85" s="9">
+        <f>SUM(B86:B90)</f>
+        <v>0</v>
+      </c>
+      <c r="C85" s="9">
+        <f>SUM(C86:C90)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B91" s="9">
+        <f>SUM(B92:B94)</f>
+        <v>0</v>
+      </c>
+      <c r="C91" s="9">
+        <f>SUM(C92:C94)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B95" s="9">
+        <f>SUM(B96:B100)</f>
+        <v>0</v>
+      </c>
+      <c r="C95" s="9">
+        <f>SUM(C96:C100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B96" s="41"/>
+      <c r="C96" s="41"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B97" s="41"/>
+      <c r="C97" s="41"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="41"/>
+      <c r="C98" s="41"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="41"/>
+      <c r="C99" s="41"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B100" s="41"/>
+      <c r="C100" s="41"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B101" s="15">
+        <f>B84</f>
+        <v>0</v>
+      </c>
+      <c r="C101" s="15">
+        <f>C84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" s="15"/>
+      <c r="C102" s="15"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B103" s="20">
+        <f>SUM(B101:B102,B83,B79)</f>
+        <v>0</v>
+      </c>
+      <c r="C103" s="20">
+        <f>SUM(C101:C102,C83,C79)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B104" s="28"/>
+      <c r="C104" s="28"/>
+    </row>
+    <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B105" s="28"/>
+      <c r="C105" s="28"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B106" s="28"/>
+      <c r="C106" s="28"/>
+    </row>
+    <row r="107" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A107" s="21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B116" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C116" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B117" s="8">
+        <f>SUM(B118:B122)</f>
+        <v>0</v>
+      </c>
+      <c r="C117" s="8">
+        <f>SUM(C118:C122)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B119" s="9"/>
+      <c r="C119" s="9"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B121" s="9"/>
+      <c r="C121" s="9"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B122" s="9">
+        <f>SUM(B123:B127)</f>
+        <v>0</v>
+      </c>
+      <c r="C122" s="9">
+        <f>SUM(C123:C127)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B124" s="10"/>
+      <c r="C124" s="10"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B125" s="10"/>
+      <c r="C125" s="10"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B126" s="10"/>
+      <c r="C126" s="10"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B128" s="8"/>
+      <c r="C128" s="8"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B129" s="8"/>
+      <c r="C129" s="8"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B130" s="8"/>
+      <c r="C130" s="8"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B131" s="16">
+        <f>SUM(B128:B130,B117)</f>
+        <v>0</v>
+      </c>
+      <c r="C131" s="16">
+        <f>SUM(C128:C130,C117)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B132" s="8">
+        <f>SUM(B133:B134)</f>
+        <v>0</v>
+      </c>
+      <c r="C132" s="8">
+        <f>SUM(C133:C134)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B133" s="10"/>
+      <c r="C133" s="10"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B134" s="10"/>
+      <c r="C134" s="10"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B135" s="16">
+        <f>B132</f>
+        <v>0</v>
+      </c>
+      <c r="C135" s="16">
+        <f>C132</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B136" s="8">
+        <f>SUM(B137,B143,B147)</f>
+        <v>0</v>
+      </c>
+      <c r="C136" s="8">
+        <f>SUM(C137,C143,C147)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B137" s="9">
+        <f>SUM(B138:B142)</f>
+        <v>0</v>
+      </c>
+      <c r="C137" s="9">
+        <f>SUM(C138:C142)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B138" s="10"/>
+      <c r="C138" s="10"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B139" s="10"/>
+      <c r="C139" s="10"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B140" s="10"/>
+      <c r="C140" s="10"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B142" s="10"/>
+      <c r="C142" s="10"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B143" s="9">
+        <f>SUM(B144:B146)</f>
+        <v>0</v>
+      </c>
+      <c r="C143" s="9">
+        <f>SUM(C144:C146)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B144" s="10"/>
+      <c r="C144" s="10"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B145" s="10"/>
+      <c r="C145" s="10"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" s="10"/>
+      <c r="C146" s="10"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B147" s="9">
+        <f>SUM(B148:B152)</f>
+        <v>0</v>
+      </c>
+      <c r="C147" s="9">
+        <f>SUM(C148:C152)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B148" s="10"/>
+      <c r="C148" s="10"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B149" s="10"/>
+      <c r="C149" s="10"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B150" s="10"/>
+      <c r="C150" s="10"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B151" s="10"/>
+      <c r="C151" s="10"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B152" s="10"/>
+      <c r="C152" s="10"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B153" s="16">
+        <f>B136</f>
+        <v>0</v>
+      </c>
+      <c r="C153" s="16">
+        <f>C136</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B154" s="16"/>
+      <c r="C154" s="16"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B155" s="16">
+        <f>SUM(B153:B154,B135,B131)</f>
+        <v>0</v>
+      </c>
+      <c r="C155" s="16">
+        <f>SUM(C153:C154,C135,C131)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B156" s="19"/>
+      <c r="C156" s="19"/>
+    </row>
+    <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B157" s="19"/>
+      <c r="C157" s="19"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B158" s="19"/>
+      <c r="C158" s="19"/>
+    </row>
+    <row r="159" spans="1:3" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B159" s="38"/>
+      <c r="C159" s="38"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B160" s="38"/>
+      <c r="C160" s="38"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B161" s="38"/>
+      <c r="C161" s="38"/>
+    </row>
+    <row r="162" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B162" s="38"/>
+      <c r="C162" s="38"/>
+    </row>
+    <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B163" s="38"/>
+      <c r="C163" s="38"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B164" s="38"/>
+      <c r="C164" s="38"/>
+    </row>
+    <row r="165" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A165" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B165" s="38"/>
+      <c r="C165" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:D35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>